<commit_message>
projeto finalizado ou quase
</commit_message>
<xml_diff>
--- a/SP Medical Group/MER/Modelo Físico.xlsx
+++ b/SP Medical Group/MER/Modelo Físico.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20354"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EB413C9-4F36-4BA6-8BCF-926E85A90364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\46962757875\Documents\Exerc-cios2-semestreSQL\SP Medical Group\MER\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46A00E1-94BF-4083-A09B-7320CE39AB4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Tipo Usuario</t>
   </si>
@@ -123,15 +118,9 @@
     <t>IdTipoUsuario</t>
   </si>
   <si>
-    <t>Telefone</t>
-  </si>
-  <si>
     <t>Clínico Geral</t>
   </si>
   <si>
-    <t>José</t>
-  </si>
-  <si>
     <t>allala</t>
   </si>
   <si>
@@ -151,13 +140,58 @@
   </si>
   <si>
     <t>Ana</t>
+  </si>
+  <si>
+    <t>Usuário</t>
+  </si>
+  <si>
+    <t>IdUsuario</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Senha</t>
+  </si>
+  <si>
+    <t>otario@gmail.com</t>
+  </si>
+  <si>
+    <t>nicolas123</t>
+  </si>
+  <si>
+    <t>cadu@gmail.com</t>
+  </si>
+  <si>
+    <t>duds@gmail.com</t>
+  </si>
+  <si>
+    <t>cadu123</t>
+  </si>
+  <si>
+    <t>duds123</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Situacao</t>
+  </si>
+  <si>
+    <t>IdSituacao</t>
+  </si>
+  <si>
+    <t>Confirmado</t>
+  </si>
+  <si>
+    <t>Aguardando</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +199,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +233,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -308,11 +368,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,9 +483,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,20 +523,56 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,7 +589,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -698,296 +885,400 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="M3:Q3"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="2"/>
-      <c r="M1" s="1" t="s">
+      <c r="D1" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="32">
+        <v>1</v>
+      </c>
+      <c r="E3" s="32">
+        <v>1</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="16" t="s">
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="38"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="32">
+        <v>2</v>
+      </c>
+      <c r="E4" s="32">
+        <v>2</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="32">
+        <v>3</v>
+      </c>
+      <c r="E5" s="32">
+        <v>3</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="41">
+        <v>1</v>
+      </c>
+      <c r="K5" s="42">
+        <v>1</v>
+      </c>
+      <c r="L5" s="42">
+        <v>1</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="43">
+        <v>43886</v>
+      </c>
+      <c r="O5" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="K8" s="28"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>2</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>3</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23">
+        <v>1</v>
+      </c>
+      <c r="F11" s="23">
+        <v>3</v>
+      </c>
+      <c r="G11" s="23">
+        <v>2</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="13">
+        <v>55555</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="11" t="s">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="8">
+        <v>12345</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="35"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>1</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="9">
-        <v>12345</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="26">
-        <v>1</v>
-      </c>
-      <c r="N3" s="27">
-        <v>1</v>
-      </c>
-      <c r="O3" s="27">
-        <v>1</v>
-      </c>
-      <c r="P3" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" s="28">
-        <v>43886</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="17">
+      <c r="E23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="17">
+      <c r="B24" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="12">
+        <v>1</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="20">
+        <v>12346</v>
+      </c>
+      <c r="G24" s="20">
+        <v>79101112</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="21">
+        <v>37112</v>
+      </c>
+      <c r="J24" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="17">
-        <v>1</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="13">
-        <v>1</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="21">
-        <v>12346</v>
-      </c>
-      <c r="G9" s="21">
-        <v>79101112</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="22">
-        <v>37112</v>
-      </c>
-      <c r="J9" s="21">
-        <v>2</v>
-      </c>
-      <c r="K9" s="23">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="17">
-        <v>2</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="17">
-        <v>3</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="D13" s="24">
-        <v>1</v>
-      </c>
-      <c r="E13" s="25">
-        <v>1</v>
-      </c>
-      <c r="F13" s="25">
-        <v>3</v>
-      </c>
-      <c r="G13" s="25">
-        <v>2</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="14">
-        <v>55555</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="7">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="J3:O3"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="D9:I9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{30A30900-7476-4D0A-88E2-EEF0559D5EA8}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{F47B83BF-A4E7-4E97-BC36-3AF797C0DF41}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{25A5CD4D-5EAB-4762-A5FC-8C203F737B1E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>